<commit_message>
add the analysis and report
</commit_message>
<xml_diff>
--- a/RP_optimization.xlsx
+++ b/RP_optimization.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Xypher\Desktop\master\高等计算机系统结构\GEMM-software-and-hardware-optimization-based-on-gem5\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{333B7C94-3B17-46B6-97CB-C1AE638E8890}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,14 +24,185 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
+  <si>
+    <t>LRU</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Random</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TreePLRU</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BIP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LIP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MRU</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LFU</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FIFO</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SecondChance</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>NRU</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>RRIP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BRRIP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gen</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hawkeye</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>run time/s</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">l1 dcache miss rate </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>l2 cache miss rate</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>5.642\%</t>
+  </si>
+  <si>
+    <t>93.2293\%</t>
+  </si>
+  <si>
+    <t>6.3317\%</t>
+  </si>
+  <si>
+    <t>82.2236\%</t>
+  </si>
+  <si>
+    <t>93.2068\%</t>
+  </si>
+  <si>
+    <t>5.4278\%</t>
+  </si>
+  <si>
+    <t>81.0817\%</t>
+  </si>
+  <si>
+    <t>5.4944\%</t>
+  </si>
+  <si>
+    <t>77.6704\%</t>
+  </si>
+  <si>
+    <t>8.7295\%</t>
+  </si>
+  <si>
+    <t>64.6209\%</t>
+  </si>
+  <si>
+    <t>7.6299\%</t>
+  </si>
+  <si>
+    <t>75.8262\%</t>
+  </si>
+  <si>
+    <t>6.3233\%</t>
+  </si>
+  <si>
+    <t>83.2052\%</t>
+  </si>
+  <si>
+    <t>5.7188\%</t>
+  </si>
+  <si>
+    <t>91.9805\%</t>
+  </si>
+  <si>
+    <t>5.5066\%</t>
+  </si>
+  <si>
+    <t>95.5215\%</t>
+  </si>
+  <si>
+    <t>5.4871\%</t>
+  </si>
+  <si>
+    <t>95.8563\%</t>
+  </si>
+  <si>
+    <t>5.3935\%</t>
+  </si>
+  <si>
+    <t>81.7344\%</t>
+  </si>
+  <si>
+    <t>7.0457\%</t>
+  </si>
+  <si>
+    <t>80.3791\%</t>
+  </si>
+  <si>
+    <t>8.7297\%</t>
+  </si>
+  <si>
+    <t>71.336\%</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="178" formatCode="0.0000%"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -46,14 +223,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="百分比" xfId="1" builtinId="5"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -330,13 +517,233 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.08203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="9" width="8.6640625" style="1"/>
+    <col min="10" max="10" width="13.08203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.6640625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.49839800000000001</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.50192899999999996</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.49837399999999998</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.46757399999999999</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.46710499999999999</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.54066599999999998</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.52578499999999995</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.50268400000000002</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.49981300000000001</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0.49682799999999999</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.49633699999999997</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0.46727600000000002</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0.51744800000000002</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0.55791400000000002</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>